<commit_message>
Clearance Rates by Region: Data Wrangling
</commit_message>
<xml_diff>
--- a/data/Crime_In_US_By_Region/Region_State.xlsx
+++ b/data/Crime_In_US_By_Region/Region_State.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dani/Documents/Datascience Projects/Website/US_Crime_Data/US_Crime_Data_Shiny/data/Crime_In_US_By_Region/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560001F6-DB71-CA49-9437-461A805F2C52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9A5769-7485-0440-A645-C6D7952B641E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="1500" windowWidth="25040" windowHeight="14500" xr2:uid="{7620E2BE-AFE8-6C4C-8566-B01FF5E78245}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="116">
   <si>
     <t>State</t>
   </si>
@@ -171,12 +171,6 @@
   </si>
   <si>
     <t>DE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     District of Columbia</t>
-  </si>
-  <si>
-    <t>DC</t>
   </si>
   <si>
     <t xml:space="preserve">     Florida</t>
@@ -824,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BC39F9D-6278-494D-BC4A-84FC626D058C}">
-  <dimension ref="A1:C103"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="86" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -846,7 +840,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -857,7 +851,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -868,7 +862,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -879,7 +873,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -890,7 +884,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -901,7 +895,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -912,7 +906,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -923,7 +917,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -934,7 +928,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -945,7 +939,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -956,7 +950,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -967,7 +961,7 @@
         <v>23</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -978,7 +972,7 @@
         <v>25</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -989,7 +983,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1000,7 +994,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1011,7 +1005,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1022,7 +1016,7 @@
         <v>33</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1033,7 +1027,7 @@
         <v>35</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1044,7 +1038,7 @@
         <v>37</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1055,7 +1049,7 @@
         <v>39</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1066,7 +1060,7 @@
         <v>41</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1077,7 +1071,7 @@
         <v>43</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1088,7 +1082,7 @@
         <v>45</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1099,7 +1093,7 @@
         <v>47</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1110,7 +1104,7 @@
         <v>49</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1121,7 +1115,7 @@
         <v>51</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1132,7 +1126,7 @@
         <v>53</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1143,7 +1137,7 @@
         <v>55</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1154,7 +1148,7 @@
         <v>57</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1165,7 +1159,7 @@
         <v>59</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1176,7 +1170,7 @@
         <v>61</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1187,7 +1181,7 @@
         <v>63</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1198,7 +1192,7 @@
         <v>65</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1209,7 +1203,7 @@
         <v>67</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1220,7 +1214,7 @@
         <v>69</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1231,7 +1225,7 @@
         <v>71</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1242,7 +1236,7 @@
         <v>73</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1253,7 +1247,7 @@
         <v>75</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1264,7 +1258,7 @@
         <v>77</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1275,7 +1269,7 @@
         <v>79</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1286,7 +1280,7 @@
         <v>81</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1297,7 +1291,7 @@
         <v>83</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1308,7 +1302,7 @@
         <v>85</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1319,7 +1313,7 @@
         <v>87</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1330,7 +1324,7 @@
         <v>89</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1341,7 +1335,7 @@
         <v>91</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1352,7 +1346,7 @@
         <v>93</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1363,7 +1357,7 @@
         <v>95</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1374,7 +1368,7 @@
         <v>97</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1385,7 +1379,7 @@
         <v>99</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1396,114 +1390,114 @@
         <v>101</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>102</v>
+        <v>2</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>106</v>
@@ -1511,131 +1505,131 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>109</v>
@@ -1643,175 +1637,175 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>113</v>
@@ -1819,10 +1813,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>113</v>
@@ -1830,145 +1824,123 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C102" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>